<commit_message>
add time to timeaccounting
</commit_message>
<xml_diff>
--- a/documentation/TimeAccounting_EECS448project3.xlsx
+++ b/documentation/TimeAccounting_EECS448project3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\Desktop\EECS448_Project3\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A946B5-4C27-4DB9-BC1D-E271DC1B54E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66621062-540A-4723-A306-99834387D909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="2258" windowWidth="12938" windowHeight="12067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7118" yWindow="2332" windowWidth="12937" windowHeight="12068" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>TEAM 02</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t xml:space="preserve">Discussion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentatiom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logic/design </t>
   </si>
 </sst>
 </file>
@@ -662,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="93" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1"/>
@@ -713,7 +722,7 @@
       </c>
       <c r="S1" s="62">
         <f>R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13</f>
-        <v>0.90486111111111123</v>
+        <v>1.3631944444444446</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
@@ -983,7 +992,9 @@
       <c r="E11" s="18">
         <v>0.55833333333333335</v>
       </c>
-      <c r="F11" s="51"/>
+      <c r="F11" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="G11" s="10"/>
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
@@ -1012,10 +1023,16 @@
       <c r="C12" s="10"/>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="H12" s="39">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I12" s="39">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="J12" s="52">
         <v>0.45833333333333331</v>
       </c>
@@ -1034,7 +1051,7 @@
       </c>
       <c r="R12" s="47">
         <f t="shared" si="1"/>
-        <v>0.63541666666666674</v>
+        <v>0.88541666666666674</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="14.25" customHeight="1">
@@ -1045,10 +1062,16 @@
       <c r="C13" s="10"/>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="H13" s="39">
+        <v>0.375</v>
+      </c>
+      <c r="I13" s="39">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="J13" s="52">
         <v>0.45833333333333331</v>
       </c>
@@ -1067,7 +1090,7 @@
       </c>
       <c r="R13" s="47">
         <f t="shared" si="1"/>
-        <v>0.15763888888888888</v>
+        <v>0.36597222222222225</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="14.25" customHeight="1">
@@ -1142,7 +1165,7 @@
       <c r="R20" s="35"/>
       <c r="S20" s="40">
         <f>(I3-H3)+(I4-H4)+(I5-H5)+(I6-H6)+(I7-H7)+(I8-H8)+(I9-H9)+(I10-H10)+(I11-H11)+(I12-H12)+(I13-H13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>4.9305555555555602E-2</v>
+        <v>0.50763888888888897</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1">
@@ -1211,7 +1234,7 @@
       <c r="R28" s="35"/>
       <c r="S28" s="45">
         <f>(I3-H3)+(I4-H4)+(I5-H5)+(I6-H6)+(I7-H7)+(I8-H8)+(I9-H9)+(I10-H10)+(I11-H11)+(I12-H12)+(I13-H13)</f>
-        <v>0</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1"/>

</xml_diff>